<commit_message>
update e-com test file + modules install
</commit_message>
<xml_diff>
--- a/bennet ecom data.xlsx
+++ b/bennet ecom data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alkemyitalia-my.sharepoint.com/personal/marco_ferracci_alkemy_com/Documents/File di Lavoro/Bennet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco.ferracci\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E49FE272-1566-49A4-A0B9-439AF7B1B641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBC0020-33EA-4EC3-8715-DB634D940259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{424AE026-9835-4B86-B82B-267CEB22A008}"/>
   </bookViews>
@@ -36,22 +36,67 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Mese di Riferimento</t>
   </si>
   <si>
     <t>Click Totali E-Com</t>
+  </si>
+  <si>
+    <t>Settembre '23</t>
+  </si>
+  <si>
+    <t>Settembre '24</t>
+  </si>
+  <si>
+    <t>Ottobre '23</t>
+  </si>
+  <si>
+    <t>Novembre '23</t>
+  </si>
+  <si>
+    <t>Dicembre '23</t>
+  </si>
+  <si>
+    <t>Gennaio '24</t>
+  </si>
+  <si>
+    <t>Febbraio '24</t>
+  </si>
+  <si>
+    <t>Marzo '24</t>
+  </si>
+  <si>
+    <t>Aprile '24</t>
+  </si>
+  <si>
+    <t>Maggio '24</t>
+  </si>
+  <si>
+    <t>Giugno '24</t>
+  </si>
+  <si>
+    <t>Luglio '24</t>
+  </si>
+  <si>
+    <t>Agosto '24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -77,8 +122,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -415,125 +469,129 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6196374-C784-413E-A709-C7A4EDBCF884}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>45170</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3">
         <v>70321</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>45200</v>
-      </c>
-      <c r="B3">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
         <v>75976</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>45231</v>
-      </c>
-      <c r="B4">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3">
         <v>79649</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>45261</v>
-      </c>
-      <c r="B5">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3">
         <v>105564</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>45292</v>
-      </c>
-      <c r="B6">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3">
         <v>85850</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>45323</v>
-      </c>
-      <c r="B7">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3">
         <v>80229</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>45352</v>
-      </c>
-      <c r="B8">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3">
         <v>96437</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>45383</v>
-      </c>
-      <c r="B9">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3">
         <v>78464</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>45413</v>
-      </c>
-      <c r="B10">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3">
         <v>83455</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>45444</v>
-      </c>
-      <c r="B11">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3">
         <v>73266</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>45474</v>
-      </c>
-      <c r="B12">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3">
         <v>77143</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>45505</v>
-      </c>
-      <c r="B13">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3">
         <v>71387</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>45536</v>
-      </c>
-      <c r="B14">
+      <c r="A14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="3">
         <v>67680</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>